<commit_message>
Commits Project Integration Resnet + Augmentation + start statistic
</commit_message>
<xml_diff>
--- a/Project 3/Onderbouwing/EDA_outcome.xlsx
+++ b/Project 3/Onderbouwing/EDA_outcome.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HansW\mitwworkspace\MakeAIWork3\Project 3\Onderbouwing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{73BE5271-25AD-4CA8-8B89-DBDAE4D05FEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D74627BB-73A9-4DE4-BE73-6D22EFFAD31D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{13DB7DE3-FFC9-433C-8E62-11A34269C583}"/>
   </bookViews>
@@ -252,13 +252,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -267,7 +266,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -585,7 +583,7 @@
   <dimension ref="B1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -602,13 +600,13 @@
       <c r="B2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="8" t="s">
         <v>20</v>
       </c>
     </row>
@@ -616,13 +614,13 @@
       <c r="B3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="3">
         <v>1</v>
       </c>
     </row>
@@ -630,13 +628,13 @@
       <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="3">
         <v>1</v>
       </c>
     </row>
@@ -644,13 +642,13 @@
       <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="3">
         <v>2</v>
       </c>
     </row>
@@ -658,13 +656,13 @@
       <c r="B6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="3">
         <v>2</v>
       </c>
     </row>
@@ -672,13 +670,13 @@
       <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="3">
         <v>2</v>
       </c>
     </row>
@@ -686,13 +684,13 @@
       <c r="B8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="3">
         <v>2</v>
       </c>
     </row>
@@ -700,11 +698,10 @@
       <c r="B9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="4">
+      <c r="E9" s="3">
         <v>3</v>
       </c>
     </row>
@@ -712,11 +709,10 @@
       <c r="B10" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="4">
+      <c r="E10" s="3">
         <v>4</v>
       </c>
     </row>
@@ -724,11 +720,10 @@
       <c r="B11" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="4">
+      <c r="E11" s="3">
         <v>4</v>
       </c>
     </row>
@@ -736,11 +731,10 @@
       <c r="B12" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="3"/>
-      <c r="E12" s="4">
+      <c r="E12" s="3">
         <v>4</v>
       </c>
     </row>
@@ -748,11 +742,10 @@
       <c r="B13" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="4">
+      <c r="E13" s="3">
         <v>4</v>
       </c>
     </row>
@@ -760,23 +753,22 @@
       <c r="B14" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="4">
+      <c r="E14" s="3">
         <v>4</v>
       </c>
     </row>
     <row r="15" spans="2:5" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="6"/>
-      <c r="E15" s="7">
+      <c r="D15" s="5"/>
+      <c r="E15" s="6">
         <v>5</v>
       </c>
     </row>

</xml_diff>